<commit_message>
Erkenntniss BCD Codierung Die Lautstärke wird nicht wie erwartet als 8 Bit Binärzahl übertragen, sondern als 2 BCD codierte Ziffern mit je 4 Bit
</commit_message>
<xml_diff>
--- a/Pulse View/Analyse.xlsx
+++ b/Pulse View/Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eigene Dateien\Hardware Tüfteleien\Smart Subwoofer\Pulse View\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5933F16E-DC20-4436-871F-F0C972C6FAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F715E94-4F27-4D91-9478-0A5A96430A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{59F7A432-8245-419D-BAF0-BDD30494A9E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{59F7A432-8245-419D-BAF0-BDD30494A9E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="31">
   <si>
     <t>E</t>
   </si>
@@ -123,9 +123,6 @@
     <t>MSB</t>
   </si>
   <si>
-    <t>LSB</t>
-  </si>
-  <si>
     <t>Div Sub</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>Diff</t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>BCD</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -430,21 +433,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -460,10 +448,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -472,6 +463,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -541,7 +546,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$Q$11,Tabelle1!$Q$18,Tabelle1!$Q$39)</c:f>
+              <c:f>(Tabelle1!$Q$12,Tabelle1!$Q$20,Tabelle1!$Q$44)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -549,10 +554,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,18 +597,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$R$11,Tabelle1!$R$18,Tabelle1!$R$39)</c:f>
+              <c:f>(Tabelle1!$R$12,Tabelle1!$R$20,Tabelle1!$R$44)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1627,6 +1632,417 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>export2!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Volume</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>export2!$A$2:$A$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>export2!$A$2:$A$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BDC7-416B-A748-3F2C4F73ABCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1770,6 +2186,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2932,13 +3379,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3358,10 +3805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F908EF-2C59-46EA-9263-539E121D3588}">
-  <dimension ref="B1:S46"/>
+  <dimension ref="B1:T52"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE23" sqref="AE23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3370,19 +3817,19 @@
     <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.85546875" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="17"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="27"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>44</v>
       </c>
@@ -3390,84 +3837,84 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-    </row>
-    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+    </row>
+    <row r="7" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14">
         <v>44</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21">
+      <c r="C8" s="15"/>
+      <c r="D8" s="16">
         <v>46</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="23"/>
-    </row>
-    <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14" t="s">
+      <c r="E9" s="21"/>
+      <c r="F9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="14" t="s">
+      <c r="I9" s="21"/>
+      <c r="J9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="14" t="s">
+      <c r="K9" s="21"/>
+      <c r="L9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="14" t="s">
+      <c r="M9" s="21"/>
+      <c r="N9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="15"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
@@ -3517,10 +3964,10 @@
         <v>15</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
@@ -3575,1008 +4022,1464 @@
         <f>R11-Q11</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+      <c r="T11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="28">
+        <f>BIN2DEC(B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="28">
+        <f t="shared" ref="C12:O12" si="0">BIN2DEC(C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="28">
+        <f>B12*10+C12</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="29">
+        <f>F12*10+G12</f>
+        <v>12</v>
+      </c>
+      <c r="S12" s="29">
+        <f>R12-Q12</f>
+        <v>12</v>
+      </c>
+      <c r="T12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-    </row>
-    <row r="14" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="19">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+    </row>
+    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="14">
         <v>44</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21">
+      <c r="C16" s="15"/>
+      <c r="D16" s="16">
         <v>46</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="23"/>
-    </row>
-    <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="24" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="18"/>
+    </row>
+    <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="14" t="s">
+      <c r="C17" s="25"/>
+      <c r="D17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="14" t="s">
+      <c r="E17" s="21"/>
+      <c r="F17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="14" t="s">
+      <c r="G17" s="21"/>
+      <c r="H17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14" t="s">
+      <c r="I17" s="21"/>
+      <c r="J17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="15"/>
-      <c r="L16" s="14" t="s">
+      <c r="K17" s="21"/>
+      <c r="L17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="15"/>
-      <c r="N16" s="14" t="s">
+      <c r="M17" s="21"/>
+      <c r="N17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="15"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="O17" s="21"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D18" s="9">
         <v>4</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E18" s="10">
         <v>5</v>
       </c>
-      <c r="F17" s="9">
-        <v>8</v>
-      </c>
-      <c r="G17" s="10">
+      <c r="F18" s="9">
+        <v>8</v>
+      </c>
+      <c r="G18" s="10">
         <v>9</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H18" s="9">
         <v>0</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I18" s="10">
         <v>1</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J18" s="9">
         <v>2</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K18" s="10">
         <v>3</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L18" s="9">
         <v>6</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M18" s="10">
         <v>7</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="N18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="O18" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="Q18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R17" s="12" t="s">
+      <c r="R18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="S17" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
+      <c r="S18" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="L19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="O19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q18" s="1">
-        <f>BIN2DEC(B18&amp;C18)</f>
+      <c r="Q19" s="1">
+        <f>BIN2DEC(B19&amp;C19)</f>
         <v>48</v>
       </c>
-      <c r="R18" s="3">
-        <f>BIN2DEC(F18&amp;G18)</f>
+      <c r="R19" s="3">
+        <f>BIN2DEC(F19&amp;G19)</f>
         <v>56</v>
       </c>
-      <c r="S18" s="2">
-        <f>R18-Q18</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="S19" s="2">
+        <f>R19-Q19</f>
+        <v>8</v>
+      </c>
+      <c r="T19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="28">
+        <f>BIN2DEC(B19)</f>
+        <v>3</v>
+      </c>
+      <c r="C20" s="28">
+        <f t="shared" ref="C20" si="1">BIN2DEC(C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="28">
+        <f t="shared" ref="D20" si="2">BIN2DEC(D19)</f>
+        <v>3</v>
+      </c>
+      <c r="E20" s="28">
+        <f t="shared" ref="E20" si="3">BIN2DEC(E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="28">
+        <f t="shared" ref="F20" si="4">BIN2DEC(F19)</f>
+        <v>3</v>
+      </c>
+      <c r="G20" s="28">
+        <f t="shared" ref="G20" si="5">BIN2DEC(G19)</f>
+        <v>8</v>
+      </c>
+      <c r="H20" s="28">
+        <f t="shared" ref="H20" si="6">BIN2DEC(H19)</f>
+        <v>3</v>
+      </c>
+      <c r="I20" s="28">
+        <f t="shared" ref="I20" si="7">BIN2DEC(I19)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="28">
+        <f t="shared" ref="J20" si="8">BIN2DEC(J19)</f>
+        <v>3</v>
+      </c>
+      <c r="K20" s="28">
+        <f t="shared" ref="K20" si="9">BIN2DEC(K19)</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="28">
+        <f t="shared" ref="L20" si="10">BIN2DEC(L19)</f>
+        <v>3</v>
+      </c>
+      <c r="M20" s="28">
+        <f t="shared" ref="M20" si="11">BIN2DEC(M19)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="28">
+        <f t="shared" ref="N20" si="12">BIN2DEC(N19)</f>
+        <v>3</v>
+      </c>
+      <c r="O20" s="28">
+        <f t="shared" ref="O20" si="13">BIN2DEC(O19)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="28">
+        <f>B20*10+C20</f>
+        <v>30</v>
+      </c>
+      <c r="R20" s="29">
+        <f>F20*10+G20</f>
+        <v>38</v>
+      </c>
+      <c r="S20" s="29">
+        <f>R20-Q20</f>
+        <v>8</v>
+      </c>
+      <c r="T20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-    </row>
-    <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="19">
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+    </row>
+    <row r="23" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="14">
         <v>44</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21">
+      <c r="C24" s="15"/>
+      <c r="D24" s="16">
         <v>46</v>
       </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="23"/>
-    </row>
-    <row r="23" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="24" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="18"/>
+    </row>
+    <row r="25" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="14" t="s">
+      <c r="C25" s="25"/>
+      <c r="D25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="26" t="s">
+      <c r="E25" s="21"/>
+      <c r="F25" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="14" t="s">
+      <c r="G25" s="23"/>
+      <c r="H25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="14" t="s">
+      <c r="I25" s="21"/>
+      <c r="J25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="14" t="s">
+      <c r="K25" s="21"/>
+      <c r="L25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="15"/>
-      <c r="N23" s="14" t="s">
+      <c r="M25" s="21"/>
+      <c r="N25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O23" s="15"/>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="O25" s="21"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D26" s="9">
         <v>4</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E26" s="10">
         <v>5</v>
       </c>
-      <c r="F24" s="9">
-        <v>8</v>
-      </c>
-      <c r="G24" s="10">
+      <c r="F26" s="9">
+        <v>8</v>
+      </c>
+      <c r="G26" s="10">
         <v>9</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H26" s="9">
         <v>0</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I26" s="10">
         <v>1</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J26" s="9">
         <v>2</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K26" s="10">
         <v>3</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L26" s="9">
         <v>6</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M26" s="10">
         <v>7</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="N26" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O24" s="10" t="s">
+      <c r="O26" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Q24" s="11" t="s">
+      <c r="Q26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R24" s="12" t="s">
+      <c r="R26" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="S24" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+      <c r="S26" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="J27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M25" s="7" t="s">
+      <c r="M27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="N27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O25" s="7" t="s">
+      <c r="O27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q25" s="1">
-        <f>BIN2DEC(B25&amp;C25)</f>
+      <c r="Q27" s="1">
+        <f>BIN2DEC(B27&amp;C27)</f>
         <v>48</v>
       </c>
-      <c r="R25" s="3">
-        <f>BIN2DEC(F25&amp;G25)</f>
+      <c r="R27" s="3">
+        <f>BIN2DEC(F27&amp;G27)</f>
         <v>49</v>
       </c>
-      <c r="S25" s="2">
-        <f>R25-Q25</f>
+      <c r="S27" s="2">
+        <f>R27-Q27</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="18" t="s">
+      <c r="T27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="28">
+        <f>BIN2DEC(B27)</f>
+        <v>3</v>
+      </c>
+      <c r="C28" s="28">
+        <f t="shared" ref="C28" si="14">BIN2DEC(C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="28">
+        <f t="shared" ref="D28" si="15">BIN2DEC(D27)</f>
+        <v>3</v>
+      </c>
+      <c r="E28" s="28">
+        <f t="shared" ref="E28" si="16">BIN2DEC(E27)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="28">
+        <f t="shared" ref="F28" si="17">BIN2DEC(F27)</f>
+        <v>3</v>
+      </c>
+      <c r="G28" s="28">
+        <f t="shared" ref="G28" si="18">BIN2DEC(G27)</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="28">
+        <f t="shared" ref="H28" si="19">BIN2DEC(H27)</f>
+        <v>3</v>
+      </c>
+      <c r="I28" s="28">
+        <f t="shared" ref="I28" si="20">BIN2DEC(I27)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="28">
+        <f t="shared" ref="J28" si="21">BIN2DEC(J27)</f>
+        <v>3</v>
+      </c>
+      <c r="K28" s="28">
+        <f t="shared" ref="K28" si="22">BIN2DEC(K27)</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="28">
+        <f t="shared" ref="L28" si="23">BIN2DEC(L27)</f>
+        <v>3</v>
+      </c>
+      <c r="M28" s="28">
+        <f t="shared" ref="M28" si="24">BIN2DEC(M27)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="28">
+        <f t="shared" ref="N28" si="25">BIN2DEC(N27)</f>
+        <v>3</v>
+      </c>
+      <c r="O28" s="28">
+        <f t="shared" ref="O28" si="26">BIN2DEC(O27)</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="28">
+        <f>B28*10+C28</f>
+        <v>30</v>
+      </c>
+      <c r="R28" s="29">
+        <f>F28*10+G28</f>
+        <v>31</v>
+      </c>
+      <c r="S28" s="29">
+        <f>R28-Q28</f>
+        <v>1</v>
+      </c>
+      <c r="T28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-    </row>
-    <row r="28" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="19">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+    </row>
+    <row r="31" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="14">
         <v>44</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21">
+      <c r="C32" s="15"/>
+      <c r="D32" s="16">
         <v>46</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="23"/>
-    </row>
-    <row r="30" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="24" t="s">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="18"/>
+    </row>
+    <row r="33" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="14" t="s">
+      <c r="C33" s="25"/>
+      <c r="D33" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="26" t="s">
+      <c r="E33" s="21"/>
+      <c r="F33" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="27"/>
-      <c r="H30" s="14" t="s">
+      <c r="G33" s="23"/>
+      <c r="H33" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="14" t="s">
+      <c r="I33" s="21"/>
+      <c r="J33" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="14" t="s">
+      <c r="K33" s="21"/>
+      <c r="L33" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M30" s="15"/>
-      <c r="N30" s="14" t="s">
+      <c r="M33" s="21"/>
+      <c r="N33" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O30" s="15"/>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="O33" s="21"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D34" s="9">
         <v>4</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E34" s="10">
         <v>5</v>
       </c>
-      <c r="F31" s="9">
-        <v>8</v>
-      </c>
-      <c r="G31" s="10">
+      <c r="F34" s="9">
+        <v>8</v>
+      </c>
+      <c r="G34" s="10">
         <v>9</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H34" s="9">
         <v>0</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I34" s="10">
         <v>1</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J34" s="9">
         <v>2</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K34" s="10">
         <v>3</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L34" s="9">
         <v>6</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M34" s="10">
         <v>7</v>
       </c>
-      <c r="N31" s="9" t="s">
+      <c r="N34" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O31" s="10" t="s">
+      <c r="O34" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Q31" s="11" t="s">
+      <c r="Q34" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R31" s="12" t="s">
+      <c r="R34" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="S31" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="6" t="s">
+      <c r="S34" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="K35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="L35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M32" s="7" t="s">
+      <c r="M35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N32" s="6" t="s">
+      <c r="N35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O32" s="7" t="s">
+      <c r="O35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q32" s="1">
-        <f>BIN2DEC(B32&amp;C32)</f>
+      <c r="Q35" s="1">
+        <f>BIN2DEC(B35&amp;C35)</f>
         <v>48</v>
       </c>
-      <c r="R32" s="3">
-        <f>BIN2DEC(F32&amp;G32)</f>
+      <c r="R35" s="3">
+        <f>BIN2DEC(F35&amp;G35)</f>
         <v>38</v>
       </c>
-      <c r="S32" s="2">
-        <f>R32-Q32</f>
+      <c r="S35" s="2">
+        <f>R35-Q35</f>
         <v>-10</v>
       </c>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+      <c r="T35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="28">
+        <f>BIN2DEC(B35)</f>
+        <v>3</v>
+      </c>
+      <c r="C36" s="28">
+        <f t="shared" ref="C36" si="27">BIN2DEC(C35)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="28">
+        <f t="shared" ref="D36" si="28">BIN2DEC(D35)</f>
+        <v>3</v>
+      </c>
+      <c r="E36" s="28">
+        <f t="shared" ref="E36" si="29">BIN2DEC(E35)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="28">
+        <f t="shared" ref="F36" si="30">BIN2DEC(F35)</f>
+        <v>2</v>
+      </c>
+      <c r="G36" s="28">
+        <f t="shared" ref="G36" si="31">BIN2DEC(G35)</f>
+        <v>6</v>
+      </c>
+      <c r="H36" s="28">
+        <f t="shared" ref="H36" si="32">BIN2DEC(H35)</f>
+        <v>3</v>
+      </c>
+      <c r="I36" s="28">
+        <f t="shared" ref="I36" si="33">BIN2DEC(I35)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="28">
+        <f t="shared" ref="J36" si="34">BIN2DEC(J35)</f>
+        <v>3</v>
+      </c>
+      <c r="K36" s="28">
+        <f t="shared" ref="K36" si="35">BIN2DEC(K35)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="28">
+        <f t="shared" ref="L36" si="36">BIN2DEC(L35)</f>
+        <v>3</v>
+      </c>
+      <c r="M36" s="28">
+        <f t="shared" ref="M36" si="37">BIN2DEC(M35)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="28">
+        <f t="shared" ref="N36" si="38">BIN2DEC(N35)</f>
+        <v>3</v>
+      </c>
+      <c r="O36" s="28">
+        <f t="shared" ref="O36" si="39">BIN2DEC(O35)</f>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="28">
+        <f>B36*10+C36</f>
+        <v>30</v>
+      </c>
+      <c r="R36" s="29">
+        <f>F36*10+G36</f>
+        <v>26</v>
+      </c>
+      <c r="S36" s="29">
+        <f>R36-Q36</f>
+        <v>-4</v>
+      </c>
+      <c r="T36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-    </row>
-    <row r="35" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="19">
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+    </row>
+    <row r="39" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="14">
         <v>44</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21">
+      <c r="C40" s="15"/>
+      <c r="D40" s="16">
         <v>46</v>
       </c>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="23"/>
-    </row>
-    <row r="37" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="24" t="s">
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="18"/>
+    </row>
+    <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="14" t="s">
+      <c r="C41" s="25"/>
+      <c r="D41" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="14" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="15"/>
-      <c r="H37" s="14" t="s">
+      <c r="G41" s="21"/>
+      <c r="H41" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="14" t="s">
+      <c r="I41" s="21"/>
+      <c r="J41" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K37" s="15"/>
-      <c r="L37" s="14" t="s">
+      <c r="K41" s="21"/>
+      <c r="L41" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="15"/>
-      <c r="N37" s="14" t="s">
+      <c r="M41" s="21"/>
+      <c r="N41" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O37" s="15"/>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+      <c r="O41" s="21"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D42" s="9">
         <v>4</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E42" s="10">
         <v>5</v>
       </c>
-      <c r="F38" s="9">
-        <v>8</v>
-      </c>
-      <c r="G38" s="10">
+      <c r="F42" s="9">
+        <v>8</v>
+      </c>
+      <c r="G42" s="10">
         <v>9</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H42" s="9">
         <v>0</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I42" s="10">
         <v>1</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J42" s="9">
         <v>2</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K42" s="10">
         <v>3</v>
       </c>
-      <c r="L38" s="9">
+      <c r="L42" s="9">
         <v>6</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M42" s="10">
         <v>7</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N42" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O38" s="10" t="s">
+      <c r="O42" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Q38" s="11" t="s">
+      <c r="Q42" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R38" s="12" t="s">
+      <c r="R42" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="S38" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="6" t="s">
+      <c r="S42" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G43" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J39" s="6" t="s">
+      <c r="J43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="K43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L39" s="6" t="s">
+      <c r="L43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M39" s="7" t="s">
+      <c r="M43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N39" s="6" t="s">
+      <c r="N43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O39" s="7" t="s">
+      <c r="O43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q39" s="1">
-        <f>BIN2DEC(B39&amp;C39)</f>
+      <c r="Q43" s="1">
+        <f>BIN2DEC(B43&amp;C43)</f>
         <v>88</v>
       </c>
-      <c r="R39" s="3">
-        <f>BIN2DEC(F39&amp;G39)</f>
+      <c r="R43" s="3">
+        <f>BIN2DEC(F43&amp;G43)</f>
         <v>102</v>
       </c>
-      <c r="S39" s="2">
-        <f>R39-Q39</f>
+      <c r="S43" s="2">
+        <f>R43-Q43</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="18" t="s">
+      <c r="T43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="28">
+        <f>BIN2DEC(B43)</f>
+        <v>5</v>
+      </c>
+      <c r="C44" s="28">
+        <f t="shared" ref="C44" si="40">BIN2DEC(C43)</f>
+        <v>8</v>
+      </c>
+      <c r="D44" s="28">
+        <f t="shared" ref="D44" si="41">BIN2DEC(D43)</f>
+        <v>5</v>
+      </c>
+      <c r="E44" s="28">
+        <f t="shared" ref="E44" si="42">BIN2DEC(E43)</f>
+        <v>8</v>
+      </c>
+      <c r="F44" s="28">
+        <f t="shared" ref="F44" si="43">BIN2DEC(F43)</f>
+        <v>6</v>
+      </c>
+      <c r="G44" s="28">
+        <f t="shared" ref="G44" si="44">BIN2DEC(G43)</f>
+        <v>6</v>
+      </c>
+      <c r="H44" s="28">
+        <f t="shared" ref="H44" si="45">BIN2DEC(H43)</f>
+        <v>5</v>
+      </c>
+      <c r="I44" s="28">
+        <f t="shared" ref="I44" si="46">BIN2DEC(I43)</f>
+        <v>8</v>
+      </c>
+      <c r="J44" s="28">
+        <f t="shared" ref="J44" si="47">BIN2DEC(J43)</f>
+        <v>5</v>
+      </c>
+      <c r="K44" s="28">
+        <f t="shared" ref="K44" si="48">BIN2DEC(K43)</f>
+        <v>8</v>
+      </c>
+      <c r="L44" s="28">
+        <f t="shared" ref="L44" si="49">BIN2DEC(L43)</f>
+        <v>5</v>
+      </c>
+      <c r="M44" s="28">
+        <f t="shared" ref="M44" si="50">BIN2DEC(M43)</f>
+        <v>8</v>
+      </c>
+      <c r="N44" s="28">
+        <f t="shared" ref="N44" si="51">BIN2DEC(N43)</f>
+        <v>5</v>
+      </c>
+      <c r="O44" s="28">
+        <f t="shared" ref="O44" si="52">BIN2DEC(O43)</f>
+        <v>8</v>
+      </c>
+      <c r="Q44" s="28">
+        <f>B44*10+C44</f>
+        <v>58</v>
+      </c>
+      <c r="R44" s="29">
+        <f>F44*10+G44</f>
+        <v>66</v>
+      </c>
+      <c r="S44" s="29">
+        <f>R44-Q44</f>
+        <v>8</v>
+      </c>
+      <c r="T44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-    </row>
-    <row r="42" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="19">
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+    </row>
+    <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="14">
         <v>44</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="21">
+      <c r="C48" s="15"/>
+      <c r="D48" s="16">
         <v>46</v>
       </c>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="23"/>
-    </row>
-    <row r="44" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="24" t="s">
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="18"/>
+    </row>
+    <row r="49" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="14" t="s">
+      <c r="C49" s="25"/>
+      <c r="D49" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="14" t="s">
+      <c r="E49" s="21"/>
+      <c r="F49" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G44" s="15"/>
-      <c r="H44" s="14" t="s">
+      <c r="G49" s="21"/>
+      <c r="H49" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="15"/>
-      <c r="J44" s="14" t="s">
+      <c r="I49" s="21"/>
+      <c r="J49" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K44" s="15"/>
-      <c r="L44" s="14" t="s">
+      <c r="K49" s="21"/>
+      <c r="L49" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M44" s="15"/>
-      <c r="N44" s="14" t="s">
+      <c r="M49" s="21"/>
+      <c r="N49" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O44" s="15"/>
-    </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="O49" s="21"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D50" s="9">
         <v>4</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E50" s="10">
         <v>5</v>
       </c>
-      <c r="F45" s="9">
-        <v>8</v>
-      </c>
-      <c r="G45" s="10">
+      <c r="F50" s="9">
+        <v>8</v>
+      </c>
+      <c r="G50" s="10">
         <v>9</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H50" s="9">
         <v>0</v>
       </c>
-      <c r="I45" s="10">
+      <c r="I50" s="10">
         <v>1</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J50" s="9">
         <v>2</v>
       </c>
-      <c r="K45" s="10">
+      <c r="K50" s="10">
         <v>3</v>
       </c>
-      <c r="L45" s="9">
+      <c r="L50" s="9">
         <v>6</v>
       </c>
-      <c r="M45" s="10">
+      <c r="M50" s="10">
         <v>7</v>
       </c>
-      <c r="N45" s="9" t="s">
+      <c r="N50" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O45" s="10" t="s">
+      <c r="O50" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Q45" s="11" t="s">
+      <c r="Q50" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R45" s="12" t="s">
+      <c r="R50" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="S45" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="6" t="s">
+      <c r="S50" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="G51" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="7" t="s">
+      <c r="I51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J46" s="6" t="s">
+      <c r="J51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K46" s="7" t="s">
+      <c r="K51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L46" s="6" t="s">
+      <c r="L51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M46" s="7" t="s">
+      <c r="M51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N46" s="6" t="s">
+      <c r="N51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O46" s="7" t="s">
+      <c r="O51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q46" s="1">
-        <f>BIN2DEC(B46&amp;C46)</f>
+      <c r="Q51" s="1">
+        <f>BIN2DEC(B51&amp;C51)</f>
         <v>118</v>
       </c>
-      <c r="R46" s="3">
-        <f>BIN2DEC(F46&amp;G46)</f>
+      <c r="R51" s="3">
+        <f>BIN2DEC(F51&amp;G51)</f>
         <v>120</v>
       </c>
-      <c r="S46" s="2">
-        <f>R46-Q46</f>
+      <c r="S51" s="2">
+        <f>R51-Q51</f>
         <v>2</v>
+      </c>
+      <c r="T51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="28">
+        <f>BIN2DEC(B51)</f>
+        <v>7</v>
+      </c>
+      <c r="C52" s="28">
+        <f t="shared" ref="C52" si="53">BIN2DEC(C51)</f>
+        <v>6</v>
+      </c>
+      <c r="D52" s="28">
+        <f t="shared" ref="D52" si="54">BIN2DEC(D51)</f>
+        <v>7</v>
+      </c>
+      <c r="E52" s="28">
+        <f t="shared" ref="E52" si="55">BIN2DEC(E51)</f>
+        <v>6</v>
+      </c>
+      <c r="F52" s="28">
+        <f t="shared" ref="F52" si="56">BIN2DEC(F51)</f>
+        <v>7</v>
+      </c>
+      <c r="G52" s="28">
+        <f t="shared" ref="G52" si="57">BIN2DEC(G51)</f>
+        <v>8</v>
+      </c>
+      <c r="H52" s="28">
+        <f t="shared" ref="H52" si="58">BIN2DEC(H51)</f>
+        <v>7</v>
+      </c>
+      <c r="I52" s="28">
+        <f t="shared" ref="I52" si="59">BIN2DEC(I51)</f>
+        <v>6</v>
+      </c>
+      <c r="J52" s="28">
+        <f t="shared" ref="J52" si="60">BIN2DEC(J51)</f>
+        <v>7</v>
+      </c>
+      <c r="K52" s="28">
+        <f t="shared" ref="K52" si="61">BIN2DEC(K51)</f>
+        <v>6</v>
+      </c>
+      <c r="L52" s="28">
+        <f t="shared" ref="L52" si="62">BIN2DEC(L51)</f>
+        <v>7</v>
+      </c>
+      <c r="M52" s="28">
+        <f t="shared" ref="M52" si="63">BIN2DEC(M51)</f>
+        <v>6</v>
+      </c>
+      <c r="N52" s="28">
+        <f t="shared" ref="N52" si="64">BIN2DEC(N51)</f>
+        <v>7</v>
+      </c>
+      <c r="O52" s="28">
+        <f t="shared" ref="O52" si="65">BIN2DEC(O51)</f>
+        <v>6</v>
+      </c>
+      <c r="Q52" s="28">
+        <f>B52*10+C52</f>
+        <v>76</v>
+      </c>
+      <c r="R52" s="29">
+        <f>F52*10+G52</f>
+        <v>78</v>
+      </c>
+      <c r="S52" s="29">
+        <f>R52-Q52</f>
+        <v>2</v>
+      </c>
+      <c r="T52" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B46:O46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:O48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:O32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B38:O38"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="D24:O24"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:O8"/>
     <mergeCell ref="B6:O6"/>
-    <mergeCell ref="B13:O13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:O15"/>
+    <mergeCell ref="B14:O14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:O16"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="B20:O20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="B34:O34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:O36"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:O43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="B27:O27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:O29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4588,21 +5491,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABE68B5-BDEF-4F44-9310-2B4792CFD757}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4617,7 +5520,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
I2C Vorbereitung - PinMode Setup vor WLAN - I2C Setup hinzugefügt - I2C Methoden angelegt - I2C noch nicht getestet - Unsicher ob ESP32 64kHz kann
</commit_message>
<xml_diff>
--- a/Pulse View/Analyse.xlsx
+++ b/Pulse View/Analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eigene Dateien\Hardware Tüfteleien\Smart Subwoofer\Pulse View\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F715E94-4F27-4D91-9478-0A5A96430A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1050F725-2D73-446D-9645-5DCBAE1FE9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{59F7A432-8245-419D-BAF0-BDD30494A9E1}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -433,6 +433,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,13 +463,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -463,20 +475,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3824,10 +3822,10 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
@@ -3846,73 +3844,73 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="B6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14">
+      <c r="B8" s="19">
         <v>44</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16">
+      <c r="C8" s="20"/>
+      <c r="D8" s="21">
         <v>46</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="18"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="23"/>
     </row>
     <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="20" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="20" t="s">
+      <c r="I9" s="15"/>
+      <c r="J9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="20" t="s">
+      <c r="K9" s="15"/>
+      <c r="L9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="20" t="s">
+      <c r="M9" s="15"/>
+      <c r="N9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="21"/>
+      <c r="O9" s="15"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -4027,71 +4025,71 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="28">
+      <c r="B12">
         <f>BIN2DEC(B11)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12">
         <f t="shared" ref="C12:O12" si="0">BIN2DEC(C11)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12" s="28">
+      <c r="M12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O12" s="28">
+      <c r="O12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="Q12">
         <f>B12*10+C12</f>
         <v>0</v>
       </c>
-      <c r="R12" s="29">
+      <c r="R12">
         <f>F12*10+G12</f>
         <v>12</v>
       </c>
-      <c r="S12" s="29">
+      <c r="S12">
         <f>R12-Q12</f>
         <v>12</v>
       </c>
@@ -4100,73 +4098,73 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
     </row>
     <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14">
+      <c r="B16" s="19">
         <v>44</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16">
+      <c r="C16" s="20"/>
+      <c r="D16" s="21">
         <v>46</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="18"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="23"/>
     </row>
     <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="25"/>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="20" t="s">
+      <c r="E17" s="15"/>
+      <c r="F17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="20" t="s">
+      <c r="G17" s="15"/>
+      <c r="H17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="20" t="s">
+      <c r="I17" s="15"/>
+      <c r="J17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="21"/>
-      <c r="L17" s="20" t="s">
+      <c r="K17" s="15"/>
+      <c r="L17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="21"/>
-      <c r="N17" s="20" t="s">
+      <c r="M17" s="15"/>
+      <c r="N17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O17" s="21"/>
+      <c r="O17" s="15"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -4281,71 +4279,71 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="28">
+      <c r="B20">
         <f>BIN2DEC(B19)</f>
         <v>3</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20">
         <f t="shared" ref="C20" si="1">BIN2DEC(C19)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20">
         <f t="shared" ref="D20" si="2">BIN2DEC(D19)</f>
         <v>3</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20">
         <f t="shared" ref="E20" si="3">BIN2DEC(E19)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20">
         <f t="shared" ref="F20" si="4">BIN2DEC(F19)</f>
         <v>3</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20">
         <f t="shared" ref="G20" si="5">BIN2DEC(G19)</f>
         <v>8</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20">
         <f t="shared" ref="H20" si="6">BIN2DEC(H19)</f>
         <v>3</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20">
         <f t="shared" ref="I20" si="7">BIN2DEC(I19)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J20">
         <f t="shared" ref="J20" si="8">BIN2DEC(J19)</f>
         <v>3</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20">
         <f t="shared" ref="K20" si="9">BIN2DEC(K19)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="28">
+      <c r="L20">
         <f t="shared" ref="L20" si="10">BIN2DEC(L19)</f>
         <v>3</v>
       </c>
-      <c r="M20" s="28">
+      <c r="M20">
         <f t="shared" ref="M20" si="11">BIN2DEC(M19)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="28">
+      <c r="N20">
         <f t="shared" ref="N20" si="12">BIN2DEC(N19)</f>
         <v>3</v>
       </c>
-      <c r="O20" s="28">
+      <c r="O20">
         <f t="shared" ref="O20" si="13">BIN2DEC(O19)</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="28">
+      <c r="Q20">
         <f>B20*10+C20</f>
         <v>30</v>
       </c>
-      <c r="R20" s="29">
+      <c r="R20">
         <f>F20*10+G20</f>
         <v>38</v>
       </c>
-      <c r="S20" s="29">
+      <c r="S20">
         <f>R20-Q20</f>
         <v>8</v>
       </c>
@@ -4370,73 +4368,73 @@
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
     </row>
     <row r="23" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14">
+      <c r="B24" s="19">
         <v>44</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16">
+      <c r="C24" s="20"/>
+      <c r="D24" s="21">
         <v>46</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="18"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="23"/>
     </row>
     <row r="25" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="25"/>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="22" t="s">
+      <c r="E25" s="15"/>
+      <c r="F25" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="20" t="s">
+      <c r="G25" s="27"/>
+      <c r="H25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="20" t="s">
+      <c r="I25" s="15"/>
+      <c r="J25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="21"/>
-      <c r="L25" s="20" t="s">
+      <c r="K25" s="15"/>
+      <c r="L25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M25" s="21"/>
-      <c r="N25" s="20" t="s">
+      <c r="M25" s="15"/>
+      <c r="N25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O25" s="21"/>
+      <c r="O25" s="15"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
@@ -4551,71 +4549,71 @@
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="28">
+      <c r="B28">
         <f>BIN2DEC(B27)</f>
         <v>3</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28">
         <f t="shared" ref="C28" si="14">BIN2DEC(C27)</f>
         <v>0</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28">
         <f t="shared" ref="D28" si="15">BIN2DEC(D27)</f>
         <v>3</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28">
         <f t="shared" ref="E28" si="16">BIN2DEC(E27)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28">
         <f t="shared" ref="F28" si="17">BIN2DEC(F27)</f>
         <v>3</v>
       </c>
-      <c r="G28" s="28">
+      <c r="G28">
         <f t="shared" ref="G28" si="18">BIN2DEC(G27)</f>
         <v>1</v>
       </c>
-      <c r="H28" s="28">
+      <c r="H28">
         <f t="shared" ref="H28" si="19">BIN2DEC(H27)</f>
         <v>3</v>
       </c>
-      <c r="I28" s="28">
+      <c r="I28">
         <f t="shared" ref="I28" si="20">BIN2DEC(I27)</f>
         <v>0</v>
       </c>
-      <c r="J28" s="28">
+      <c r="J28">
         <f t="shared" ref="J28" si="21">BIN2DEC(J27)</f>
         <v>3</v>
       </c>
-      <c r="K28" s="28">
+      <c r="K28">
         <f t="shared" ref="K28" si="22">BIN2DEC(K27)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="28">
+      <c r="L28">
         <f t="shared" ref="L28" si="23">BIN2DEC(L27)</f>
         <v>3</v>
       </c>
-      <c r="M28" s="28">
+      <c r="M28">
         <f t="shared" ref="M28" si="24">BIN2DEC(M27)</f>
         <v>0</v>
       </c>
-      <c r="N28" s="28">
+      <c r="N28">
         <f t="shared" ref="N28" si="25">BIN2DEC(N27)</f>
         <v>3</v>
       </c>
-      <c r="O28" s="28">
+      <c r="O28">
         <f t="shared" ref="O28" si="26">BIN2DEC(O27)</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="28">
+      <c r="Q28">
         <f>B28*10+C28</f>
         <v>30</v>
       </c>
-      <c r="R28" s="29">
+      <c r="R28">
         <f>F28*10+G28</f>
         <v>31</v>
       </c>
-      <c r="S28" s="29">
+      <c r="S28">
         <f>R28-Q28</f>
         <v>1</v>
       </c>
@@ -4640,73 +4638,73 @@
       <c r="O29" s="8"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
     </row>
     <row r="31" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14">
+      <c r="B32" s="19">
         <v>44</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16">
+      <c r="C32" s="20"/>
+      <c r="D32" s="21">
         <v>46</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="18"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="23"/>
     </row>
     <row r="33" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="25"/>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="22" t="s">
+      <c r="E33" s="15"/>
+      <c r="F33" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="20" t="s">
+      <c r="G33" s="27"/>
+      <c r="H33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="20" t="s">
+      <c r="I33" s="15"/>
+      <c r="J33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="21"/>
-      <c r="L33" s="20" t="s">
+      <c r="K33" s="15"/>
+      <c r="L33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M33" s="21"/>
-      <c r="N33" s="20" t="s">
+      <c r="M33" s="15"/>
+      <c r="N33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O33" s="21"/>
+      <c r="O33" s="15"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -4821,71 +4819,71 @@
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="28">
+      <c r="B36">
         <f>BIN2DEC(B35)</f>
         <v>3</v>
       </c>
-      <c r="C36" s="28">
+      <c r="C36">
         <f t="shared" ref="C36" si="27">BIN2DEC(C35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36">
         <f t="shared" ref="D36" si="28">BIN2DEC(D35)</f>
         <v>3</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36">
         <f t="shared" ref="E36" si="29">BIN2DEC(E35)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36">
         <f t="shared" ref="F36" si="30">BIN2DEC(F35)</f>
         <v>2</v>
       </c>
-      <c r="G36" s="28">
+      <c r="G36">
         <f t="shared" ref="G36" si="31">BIN2DEC(G35)</f>
         <v>6</v>
       </c>
-      <c r="H36" s="28">
+      <c r="H36">
         <f t="shared" ref="H36" si="32">BIN2DEC(H35)</f>
         <v>3</v>
       </c>
-      <c r="I36" s="28">
+      <c r="I36">
         <f t="shared" ref="I36" si="33">BIN2DEC(I35)</f>
         <v>0</v>
       </c>
-      <c r="J36" s="28">
+      <c r="J36">
         <f t="shared" ref="J36" si="34">BIN2DEC(J35)</f>
         <v>3</v>
       </c>
-      <c r="K36" s="28">
+      <c r="K36">
         <f t="shared" ref="K36" si="35">BIN2DEC(K35)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="28">
+      <c r="L36">
         <f t="shared" ref="L36" si="36">BIN2DEC(L35)</f>
         <v>3</v>
       </c>
-      <c r="M36" s="28">
+      <c r="M36">
         <f t="shared" ref="M36" si="37">BIN2DEC(M35)</f>
         <v>0</v>
       </c>
-      <c r="N36" s="28">
+      <c r="N36">
         <f t="shared" ref="N36" si="38">BIN2DEC(N35)</f>
         <v>3</v>
       </c>
-      <c r="O36" s="28">
+      <c r="O36">
         <f t="shared" ref="O36" si="39">BIN2DEC(O35)</f>
         <v>0</v>
       </c>
-      <c r="Q36" s="28">
+      <c r="Q36">
         <f>B36*10+C36</f>
         <v>30</v>
       </c>
-      <c r="R36" s="29">
+      <c r="R36">
         <f>F36*10+G36</f>
         <v>26</v>
       </c>
-      <c r="S36" s="29">
+      <c r="S36">
         <f>R36-Q36</f>
         <v>-4</v>
       </c>
@@ -4910,73 +4908,73 @@
       <c r="O37" s="8"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
     </row>
     <row r="39" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="14">
+      <c r="B40" s="19">
         <v>44</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="16">
+      <c r="C40" s="20"/>
+      <c r="D40" s="21">
         <v>46</v>
       </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="18"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="23"/>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="25"/>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="20" t="s">
+      <c r="E41" s="15"/>
+      <c r="F41" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="21"/>
-      <c r="H41" s="20" t="s">
+      <c r="G41" s="15"/>
+      <c r="H41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="20" t="s">
+      <c r="I41" s="15"/>
+      <c r="J41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K41" s="21"/>
-      <c r="L41" s="20" t="s">
+      <c r="K41" s="15"/>
+      <c r="L41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M41" s="21"/>
-      <c r="N41" s="20" t="s">
+      <c r="M41" s="15"/>
+      <c r="N41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O41" s="21"/>
+      <c r="O41" s="15"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
@@ -5091,71 +5089,71 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="28">
+      <c r="B44">
         <f>BIN2DEC(B43)</f>
         <v>5</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C44">
         <f t="shared" ref="C44" si="40">BIN2DEC(C43)</f>
         <v>8</v>
       </c>
-      <c r="D44" s="28">
+      <c r="D44">
         <f t="shared" ref="D44" si="41">BIN2DEC(D43)</f>
         <v>5</v>
       </c>
-      <c r="E44" s="28">
+      <c r="E44">
         <f t="shared" ref="E44" si="42">BIN2DEC(E43)</f>
         <v>8</v>
       </c>
-      <c r="F44" s="28">
+      <c r="F44">
         <f t="shared" ref="F44" si="43">BIN2DEC(F43)</f>
         <v>6</v>
       </c>
-      <c r="G44" s="28">
+      <c r="G44">
         <f t="shared" ref="G44" si="44">BIN2DEC(G43)</f>
         <v>6</v>
       </c>
-      <c r="H44" s="28">
+      <c r="H44">
         <f t="shared" ref="H44" si="45">BIN2DEC(H43)</f>
         <v>5</v>
       </c>
-      <c r="I44" s="28">
+      <c r="I44">
         <f t="shared" ref="I44" si="46">BIN2DEC(I43)</f>
         <v>8</v>
       </c>
-      <c r="J44" s="28">
+      <c r="J44">
         <f t="shared" ref="J44" si="47">BIN2DEC(J43)</f>
         <v>5</v>
       </c>
-      <c r="K44" s="28">
+      <c r="K44">
         <f t="shared" ref="K44" si="48">BIN2DEC(K43)</f>
         <v>8</v>
       </c>
-      <c r="L44" s="28">
+      <c r="L44">
         <f t="shared" ref="L44" si="49">BIN2DEC(L43)</f>
         <v>5</v>
       </c>
-      <c r="M44" s="28">
+      <c r="M44">
         <f t="shared" ref="M44" si="50">BIN2DEC(M43)</f>
         <v>8</v>
       </c>
-      <c r="N44" s="28">
+      <c r="N44">
         <f t="shared" ref="N44" si="51">BIN2DEC(N43)</f>
         <v>5</v>
       </c>
-      <c r="O44" s="28">
+      <c r="O44">
         <f t="shared" ref="O44" si="52">BIN2DEC(O43)</f>
         <v>8</v>
       </c>
-      <c r="Q44" s="28">
+      <c r="Q44">
         <f>B44*10+C44</f>
         <v>58</v>
       </c>
-      <c r="R44" s="29">
+      <c r="R44">
         <f>F44*10+G44</f>
         <v>66</v>
       </c>
-      <c r="S44" s="29">
+      <c r="S44">
         <f>R44-Q44</f>
         <v>8</v>
       </c>
@@ -5164,73 +5162,73 @@
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="14">
+      <c r="B48" s="19">
         <v>44</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="16">
+      <c r="C48" s="20"/>
+      <c r="D48" s="21">
         <v>46</v>
       </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="17"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="18"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
+      <c r="N48" s="22"/>
+      <c r="O48" s="23"/>
     </row>
     <row r="49" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C49" s="25"/>
-      <c r="D49" s="20" t="s">
+      <c r="D49" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="21"/>
-      <c r="F49" s="20" t="s">
+      <c r="E49" s="15"/>
+      <c r="F49" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G49" s="21"/>
-      <c r="H49" s="20" t="s">
+      <c r="G49" s="15"/>
+      <c r="H49" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I49" s="21"/>
-      <c r="J49" s="20" t="s">
+      <c r="I49" s="15"/>
+      <c r="J49" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K49" s="21"/>
-      <c r="L49" s="20" t="s">
+      <c r="K49" s="15"/>
+      <c r="L49" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M49" s="21"/>
-      <c r="N49" s="20" t="s">
+      <c r="M49" s="15"/>
+      <c r="N49" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O49" s="21"/>
+      <c r="O49" s="15"/>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
@@ -5345,71 +5343,71 @@
       </c>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B52" s="28">
+      <c r="B52">
         <f>BIN2DEC(B51)</f>
         <v>7</v>
       </c>
-      <c r="C52" s="28">
+      <c r="C52">
         <f t="shared" ref="C52" si="53">BIN2DEC(C51)</f>
         <v>6</v>
       </c>
-      <c r="D52" s="28">
+      <c r="D52">
         <f t="shared" ref="D52" si="54">BIN2DEC(D51)</f>
         <v>7</v>
       </c>
-      <c r="E52" s="28">
+      <c r="E52">
         <f t="shared" ref="E52" si="55">BIN2DEC(E51)</f>
         <v>6</v>
       </c>
-      <c r="F52" s="28">
+      <c r="F52">
         <f t="shared" ref="F52" si="56">BIN2DEC(F51)</f>
         <v>7</v>
       </c>
-      <c r="G52" s="28">
+      <c r="G52">
         <f t="shared" ref="G52" si="57">BIN2DEC(G51)</f>
         <v>8</v>
       </c>
-      <c r="H52" s="28">
+      <c r="H52">
         <f t="shared" ref="H52" si="58">BIN2DEC(H51)</f>
         <v>7</v>
       </c>
-      <c r="I52" s="28">
+      <c r="I52">
         <f t="shared" ref="I52" si="59">BIN2DEC(I51)</f>
         <v>6</v>
       </c>
-      <c r="J52" s="28">
+      <c r="J52">
         <f t="shared" ref="J52" si="60">BIN2DEC(J51)</f>
         <v>7</v>
       </c>
-      <c r="K52" s="28">
+      <c r="K52">
         <f t="shared" ref="K52" si="61">BIN2DEC(K51)</f>
         <v>6</v>
       </c>
-      <c r="L52" s="28">
+      <c r="L52">
         <f t="shared" ref="L52" si="62">BIN2DEC(L51)</f>
         <v>7</v>
       </c>
-      <c r="M52" s="28">
+      <c r="M52">
         <f t="shared" ref="M52" si="63">BIN2DEC(M51)</f>
         <v>6</v>
       </c>
-      <c r="N52" s="28">
+      <c r="N52">
         <f t="shared" ref="N52" si="64">BIN2DEC(N51)</f>
         <v>7</v>
       </c>
-      <c r="O52" s="28">
+      <c r="O52">
         <f t="shared" ref="O52" si="65">BIN2DEC(O51)</f>
         <v>6</v>
       </c>
-      <c r="Q52" s="28">
+      <c r="Q52">
         <f>B52*10+C52</f>
         <v>76</v>
       </c>
-      <c r="R52" s="29">
+      <c r="R52">
         <f>F52*10+G52</f>
         <v>78</v>
       </c>
-      <c r="S52" s="29">
+      <c r="S52">
         <f>R52-Q52</f>
         <v>2</v>
       </c>
@@ -5419,6 +5417,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="B6:O6"/>
+    <mergeCell ref="B14:O14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:O16"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="D24:O24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B38:O38"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="N49:O49"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B46:O46"/>
@@ -5435,51 +5478,6 @@
     <mergeCell ref="D32:O32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B38:O38"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:O40"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="B6:O6"/>
-    <mergeCell ref="B14:O14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>